<commit_message>
Updated Req and Design docs, adding Lawrence to authors.
</commit_message>
<xml_diff>
--- a/design/MIDI-Freq-Table.xlsx
+++ b/design/MIDI-Freq-Table.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielb/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielb/github.com/daniel-birket/audible-plot/design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3DBC845-D653-9B4D-AA66-F1FA57F3F7EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1937A027-35C6-9743-9B1C-B4C981865402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3840" yWindow="2200" windowWidth="28100" windowHeight="17440" xr2:uid="{6F333C22-56D9-A842-932D-AF299D6421EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="17">
   <si>
     <t>MIDI</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>NoteOct</t>
   </si>
 </sst>
 </file>
@@ -443,15 +446,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E95D5295-EBC7-0B40-AFE9-3291C306EFAF}">
-  <dimension ref="A1:D129"/>
+  <dimension ref="A1:E129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="D121" sqref="D121"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14:E129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -464,8 +467,11 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -481,7 +487,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -497,7 +503,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -513,7 +519,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -529,7 +535,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -545,7 +551,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -561,7 +567,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -577,7 +583,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -593,7 +599,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -609,7 +615,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -625,7 +631,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -641,7 +647,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -657,7 +663,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -672,8 +678,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" t="str">
+        <f>C14&amp;D14</f>
+        <v>C0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -688,8 +698,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" t="str">
+        <f t="shared" ref="E15:E78" si="2">C15&amp;D15</f>
+        <v>C#0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -704,8 +718,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" t="str">
+        <f t="shared" si="2"/>
+        <v>D0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -720,8 +738,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" t="str">
+        <f t="shared" si="2"/>
+        <v>D#0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -736,8 +758,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" t="str">
+        <f t="shared" si="2"/>
+        <v>E0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -752,8 +778,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" t="str">
+        <f t="shared" si="2"/>
+        <v>F0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -768,8 +798,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" t="str">
+        <f t="shared" si="2"/>
+        <v>F#0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -784,8 +818,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" t="str">
+        <f t="shared" si="2"/>
+        <v>G0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -800,8 +838,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" t="str">
+        <f t="shared" si="2"/>
+        <v>G#0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -816,8 +858,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" t="str">
+        <f t="shared" si="2"/>
+        <v>A0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -832,8 +878,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" t="str">
+        <f t="shared" si="2"/>
+        <v>A#0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -848,8 +898,12 @@
         <f>D37-1</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" t="str">
+        <f t="shared" si="2"/>
+        <v>B0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -863,8 +917,12 @@
       <c r="D26" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" t="str">
+        <f t="shared" si="2"/>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -878,8 +936,12 @@
       <c r="D27" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" t="str">
+        <f t="shared" si="2"/>
+        <v>C#1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -893,8 +955,12 @@
       <c r="D28" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" t="str">
+        <f t="shared" si="2"/>
+        <v>D1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -908,8 +974,12 @@
       <c r="D29" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" t="str">
+        <f t="shared" si="2"/>
+        <v>D#1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -923,8 +993,12 @@
       <c r="D30" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" t="str">
+        <f t="shared" si="2"/>
+        <v>E1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -938,8 +1012,12 @@
       <c r="D31" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" t="str">
+        <f t="shared" si="2"/>
+        <v>F1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -953,8 +1031,12 @@
       <c r="D32" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" t="str">
+        <f t="shared" si="2"/>
+        <v>F#1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
@@ -968,8 +1050,12 @@
       <c r="D33" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" t="str">
+        <f t="shared" si="2"/>
+        <v>G1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
@@ -983,8 +1069,12 @@
       <c r="D34" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" t="str">
+        <f t="shared" si="2"/>
+        <v>G#1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
@@ -998,8 +1088,12 @@
       <c r="D35" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35" t="str">
+        <f t="shared" si="2"/>
+        <v>A1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
@@ -1013,8 +1107,12 @@
       <c r="D36" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" t="str">
+        <f t="shared" si="2"/>
+        <v>A#1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
@@ -1028,8 +1126,12 @@
       <c r="D37" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" t="str">
+        <f t="shared" si="2"/>
+        <v>B1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
@@ -1044,8 +1146,12 @@
         <f>D26+1</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" t="str">
+        <f t="shared" si="2"/>
+        <v>C2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
@@ -1057,11 +1163,15 @@
         <v>5</v>
       </c>
       <c r="D39">
-        <f t="shared" ref="D39:D102" si="2">D27+1</f>
+        <f t="shared" ref="D39:D102" si="3">D27+1</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" t="str">
+        <f t="shared" si="2"/>
+        <v>C#2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
@@ -1073,11 +1183,15 @@
         <v>6</v>
       </c>
       <c r="D40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40" t="str">
+        <f t="shared" si="2"/>
+        <v>D2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
@@ -1089,11 +1203,15 @@
         <v>7</v>
       </c>
       <c r="D41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41" t="str">
+        <f t="shared" si="2"/>
+        <v>D#2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
@@ -1105,11 +1223,15 @@
         <v>8</v>
       </c>
       <c r="D42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42" t="str">
+        <f t="shared" si="2"/>
+        <v>E2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
@@ -1121,11 +1243,15 @@
         <v>9</v>
       </c>
       <c r="D43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43" t="str">
+        <f t="shared" si="2"/>
+        <v>F2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
@@ -1137,11 +1263,15 @@
         <v>10</v>
       </c>
       <c r="D44">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44" t="str">
+        <f t="shared" si="2"/>
+        <v>F#2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
@@ -1153,11 +1283,15 @@
         <v>11</v>
       </c>
       <c r="D45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45" t="str">
+        <f t="shared" si="2"/>
+        <v>G2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
@@ -1169,11 +1303,15 @@
         <v>12</v>
       </c>
       <c r="D46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46" t="str">
+        <f t="shared" si="2"/>
+        <v>G#2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
@@ -1185,11 +1323,15 @@
         <v>13</v>
       </c>
       <c r="D47">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47" t="str">
+        <f t="shared" si="2"/>
+        <v>A2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
@@ -1201,11 +1343,15 @@
         <v>14</v>
       </c>
       <c r="D48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48" t="str">
+        <f t="shared" si="2"/>
+        <v>A#2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>47</v>
       </c>
@@ -1217,11 +1363,15 @@
         <v>15</v>
       </c>
       <c r="D49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49" t="str">
+        <f t="shared" si="2"/>
+        <v>B2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>48</v>
       </c>
@@ -1233,11 +1383,15 @@
         <v>4</v>
       </c>
       <c r="D50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50" t="str">
+        <f t="shared" si="2"/>
+        <v>C3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49</v>
       </c>
@@ -1249,11 +1403,15 @@
         <v>5</v>
       </c>
       <c r="D51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51" t="str">
+        <f t="shared" si="2"/>
+        <v>C#3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>50</v>
       </c>
@@ -1265,11 +1423,15 @@
         <v>6</v>
       </c>
       <c r="D52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52" t="str">
+        <f t="shared" si="2"/>
+        <v>D3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>51</v>
       </c>
@@ -1281,11 +1443,15 @@
         <v>7</v>
       </c>
       <c r="D53">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53" t="str">
+        <f t="shared" si="2"/>
+        <v>D#3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>52</v>
       </c>
@@ -1297,11 +1463,15 @@
         <v>8</v>
       </c>
       <c r="D54">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E54" t="str">
+        <f t="shared" si="2"/>
+        <v>E3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>53</v>
       </c>
@@ -1313,11 +1483,15 @@
         <v>9</v>
       </c>
       <c r="D55">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E55" t="str">
+        <f t="shared" si="2"/>
+        <v>F3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>54</v>
       </c>
@@ -1329,11 +1503,15 @@
         <v>10</v>
       </c>
       <c r="D56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56" t="str">
+        <f t="shared" si="2"/>
+        <v>F#3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>55</v>
       </c>
@@ -1345,11 +1523,15 @@
         <v>11</v>
       </c>
       <c r="D57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57" t="str">
+        <f t="shared" si="2"/>
+        <v>G3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>56</v>
       </c>
@@ -1361,11 +1543,15 @@
         <v>12</v>
       </c>
       <c r="D58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58" t="str">
+        <f t="shared" si="2"/>
+        <v>G#3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>57</v>
       </c>
@@ -1377,11 +1563,15 @@
         <v>13</v>
       </c>
       <c r="D59">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59" t="str">
+        <f t="shared" si="2"/>
+        <v>A3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>58</v>
       </c>
@@ -1393,11 +1583,15 @@
         <v>14</v>
       </c>
       <c r="D60">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60" t="str">
+        <f t="shared" si="2"/>
+        <v>A#3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>59</v>
       </c>
@@ -1409,11 +1603,15 @@
         <v>15</v>
       </c>
       <c r="D61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61" t="str">
+        <f t="shared" si="2"/>
+        <v>B3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>60</v>
       </c>
@@ -1425,11 +1623,15 @@
         <v>4</v>
       </c>
       <c r="D62">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E62" t="str">
+        <f t="shared" si="2"/>
+        <v>C4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>61</v>
       </c>
@@ -1441,11 +1643,15 @@
         <v>5</v>
       </c>
       <c r="D63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E63" t="str">
+        <f t="shared" si="2"/>
+        <v>C#4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>62</v>
       </c>
@@ -1457,11 +1663,15 @@
         <v>6</v>
       </c>
       <c r="D64">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E64" t="str">
+        <f t="shared" si="2"/>
+        <v>D4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>63</v>
       </c>
@@ -1473,11 +1683,15 @@
         <v>7</v>
       </c>
       <c r="D65">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65" t="str">
+        <f t="shared" si="2"/>
+        <v>D#4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>64</v>
       </c>
@@ -1489,75 +1703,95 @@
         <v>8</v>
       </c>
       <c r="D66">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66" t="str">
+        <f t="shared" si="2"/>
+        <v>E4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>65</v>
       </c>
       <c r="B67" s="1">
-        <f t="shared" ref="B67:B129" si="3">2^((A67-A$71)/12)*B$71</f>
+        <f t="shared" ref="B67:B129" si="4">2^((A67-A$71)/12)*B$71</f>
         <v>349.22823143300388</v>
       </c>
       <c r="C67" t="s">
         <v>9</v>
       </c>
       <c r="D67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E67" t="str">
+        <f t="shared" si="2"/>
+        <v>F4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>66</v>
       </c>
       <c r="B68" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>369.99442271163446</v>
       </c>
       <c r="C68" t="s">
         <v>10</v>
       </c>
       <c r="D68">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E68" t="str">
+        <f t="shared" si="2"/>
+        <v>F#4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>67</v>
       </c>
       <c r="B69" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>391.99543598174927</v>
       </c>
       <c r="C69" t="s">
         <v>11</v>
       </c>
       <c r="D69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E69" t="str">
+        <f t="shared" si="2"/>
+        <v>G4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>68</v>
       </c>
       <c r="B70" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>415.30469757994513</v>
       </c>
       <c r="C70" t="s">
         <v>12</v>
       </c>
       <c r="D70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E70" t="str">
+        <f t="shared" si="2"/>
+        <v>G#4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>69</v>
       </c>
@@ -1568,640 +1802,800 @@
         <v>13</v>
       </c>
       <c r="D71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E71" t="str">
+        <f t="shared" si="2"/>
+        <v>A4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>70</v>
       </c>
       <c r="B72" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>466.16376151808993</v>
       </c>
       <c r="C72" t="s">
         <v>14</v>
       </c>
       <c r="D72">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E72" t="str">
+        <f t="shared" si="2"/>
+        <v>A#4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>71</v>
       </c>
       <c r="B73" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>493.88330125612413</v>
       </c>
       <c r="C73" t="s">
         <v>15</v>
       </c>
       <c r="D73">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E73" t="str">
+        <f t="shared" si="2"/>
+        <v>B4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>72</v>
       </c>
       <c r="B74" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>523.25113060119725</v>
       </c>
       <c r="C74" t="s">
         <v>4</v>
       </c>
       <c r="D74">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E74" t="str">
+        <f t="shared" si="2"/>
+        <v>C5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>73</v>
       </c>
       <c r="B75" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>554.36526195374415</v>
       </c>
       <c r="C75" t="s">
         <v>5</v>
       </c>
       <c r="D75">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E75" t="str">
+        <f t="shared" si="2"/>
+        <v>C#5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>74</v>
       </c>
       <c r="B76" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>587.32953583481515</v>
       </c>
       <c r="C76" t="s">
         <v>6</v>
       </c>
       <c r="D76">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E76" t="str">
+        <f t="shared" si="2"/>
+        <v>D5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>75</v>
       </c>
       <c r="B77" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>622.25396744416184</v>
       </c>
       <c r="C77" t="s">
         <v>7</v>
       </c>
       <c r="D77">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E77" t="str">
+        <f t="shared" si="2"/>
+        <v>D#5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>76</v>
       </c>
       <c r="B78" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>659.25511382573984</v>
       </c>
       <c r="C78" t="s">
         <v>8</v>
       </c>
       <c r="D78">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E78" t="str">
+        <f t="shared" si="2"/>
+        <v>E5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>77</v>
       </c>
       <c r="B79" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>698.45646286600777</v>
       </c>
       <c r="C79" t="s">
         <v>9</v>
       </c>
       <c r="D79">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E79" t="str">
+        <f t="shared" ref="E79:E129" si="5">C79&amp;D79</f>
+        <v>F5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>78</v>
       </c>
       <c r="B80" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>739.9888454232688</v>
       </c>
       <c r="C80" t="s">
         <v>10</v>
       </c>
       <c r="D80">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E80" t="str">
+        <f t="shared" si="5"/>
+        <v>F#5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>79</v>
       </c>
       <c r="B81" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>783.99087196349853</v>
       </c>
       <c r="C81" t="s">
         <v>11</v>
       </c>
       <c r="D81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E81" t="str">
+        <f t="shared" si="5"/>
+        <v>G5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>80</v>
       </c>
       <c r="B82" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>830.60939515989025</v>
       </c>
       <c r="C82" t="s">
         <v>12</v>
       </c>
       <c r="D82">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E82" t="str">
+        <f t="shared" si="5"/>
+        <v>G#5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>81</v>
       </c>
       <c r="B83" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>880</v>
       </c>
       <c r="C83" t="s">
         <v>13</v>
       </c>
       <c r="D83">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E83" t="str">
+        <f t="shared" si="5"/>
+        <v>A5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>82</v>
       </c>
       <c r="B84" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>932.32752303617963</v>
       </c>
       <c r="C84" t="s">
         <v>14</v>
       </c>
       <c r="D84">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E84" t="str">
+        <f t="shared" si="5"/>
+        <v>A#5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>83</v>
       </c>
       <c r="B85" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>987.76660251224826</v>
       </c>
       <c r="C85" t="s">
         <v>15</v>
       </c>
       <c r="D85">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E85" t="str">
+        <f t="shared" si="5"/>
+        <v>B5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>84</v>
       </c>
       <c r="B86" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1046.5022612023945</v>
       </c>
       <c r="C86" t="s">
         <v>4</v>
       </c>
       <c r="D86">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E86" t="str">
+        <f t="shared" si="5"/>
+        <v>C6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>85</v>
       </c>
       <c r="B87" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1108.7305239074883</v>
       </c>
       <c r="C87" t="s">
         <v>5</v>
       </c>
       <c r="D87">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E87" t="str">
+        <f t="shared" si="5"/>
+        <v>C#6</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>86</v>
       </c>
       <c r="B88" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1174.6590716696303</v>
       </c>
       <c r="C88" t="s">
         <v>6</v>
       </c>
       <c r="D88">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E88" t="str">
+        <f t="shared" si="5"/>
+        <v>D6</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>87</v>
       </c>
       <c r="B89" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1244.5079348883235</v>
       </c>
       <c r="C89" t="s">
         <v>7</v>
       </c>
       <c r="D89">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E89" t="str">
+        <f t="shared" si="5"/>
+        <v>D#6</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>88</v>
       </c>
       <c r="B90" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1318.5102276514795</v>
       </c>
       <c r="C90" t="s">
         <v>8</v>
       </c>
       <c r="D90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E90" t="str">
+        <f t="shared" si="5"/>
+        <v>E6</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>89</v>
       </c>
       <c r="B91" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1396.9129257320155</v>
       </c>
       <c r="C91" t="s">
         <v>9</v>
       </c>
       <c r="D91">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E91" t="str">
+        <f t="shared" si="5"/>
+        <v>F6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>90</v>
       </c>
       <c r="B92" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1479.9776908465376</v>
       </c>
       <c r="C92" t="s">
         <v>10</v>
       </c>
       <c r="D92">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E92" t="str">
+        <f t="shared" si="5"/>
+        <v>F#6</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>91</v>
       </c>
       <c r="B93" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1567.9817439269968</v>
       </c>
       <c r="C93" t="s">
         <v>11</v>
       </c>
       <c r="D93">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E93" t="str">
+        <f t="shared" si="5"/>
+        <v>G6</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>92</v>
       </c>
       <c r="B94" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1661.2187903197805</v>
       </c>
       <c r="C94" t="s">
         <v>12</v>
       </c>
       <c r="D94">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E94" t="str">
+        <f t="shared" si="5"/>
+        <v>G#6</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>93</v>
       </c>
       <c r="B95" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1760</v>
       </c>
       <c r="C95" t="s">
         <v>13</v>
       </c>
       <c r="D95">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E95" t="str">
+        <f t="shared" si="5"/>
+        <v>A6</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>94</v>
       </c>
       <c r="B96" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1864.6550460723597</v>
       </c>
       <c r="C96" t="s">
         <v>14</v>
       </c>
       <c r="D96">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E96" t="str">
+        <f t="shared" si="5"/>
+        <v>A#6</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>95</v>
       </c>
       <c r="B97" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1975.5332050244961</v>
       </c>
       <c r="C97" t="s">
         <v>15</v>
       </c>
       <c r="D97">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E97" t="str">
+        <f t="shared" si="5"/>
+        <v>B6</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>96</v>
       </c>
       <c r="B98" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2093.004522404789</v>
       </c>
       <c r="C98" t="s">
         <v>4</v>
       </c>
       <c r="D98">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E98" t="str">
+        <f t="shared" si="5"/>
+        <v>C7</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>97</v>
       </c>
       <c r="B99" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2217.4610478149771</v>
       </c>
       <c r="C99" t="s">
         <v>5</v>
       </c>
       <c r="D99">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E99" t="str">
+        <f t="shared" si="5"/>
+        <v>C#7</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>98</v>
       </c>
       <c r="B100" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2349.3181433392601</v>
       </c>
       <c r="C100" t="s">
         <v>6</v>
       </c>
       <c r="D100">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E100" t="str">
+        <f t="shared" si="5"/>
+        <v>D7</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>99</v>
       </c>
       <c r="B101" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2489.0158697766474</v>
       </c>
       <c r="C101" t="s">
         <v>7</v>
       </c>
       <c r="D101">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E101" t="str">
+        <f t="shared" si="5"/>
+        <v>D#7</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>100</v>
       </c>
       <c r="B102" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2637.0204553029598</v>
       </c>
       <c r="C102" t="s">
         <v>8</v>
       </c>
       <c r="D102">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E102" t="str">
+        <f t="shared" si="5"/>
+        <v>E7</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>101</v>
       </c>
       <c r="B103" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2793.8258514640311</v>
       </c>
       <c r="C103" t="s">
         <v>9</v>
       </c>
       <c r="D103">
-        <f t="shared" ref="D103:D110" si="4">D91+1</f>
+        <f t="shared" ref="D103:D110" si="6">D91+1</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E103" t="str">
+        <f t="shared" si="5"/>
+        <v>F7</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>102</v>
       </c>
       <c r="B104" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2959.9553816930757</v>
       </c>
       <c r="C104" t="s">
         <v>10</v>
       </c>
       <c r="D104">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E104" t="str">
+        <f t="shared" si="5"/>
+        <v>F#7</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>103</v>
       </c>
       <c r="B105" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3135.9634878539941</v>
       </c>
       <c r="C105" t="s">
         <v>11</v>
       </c>
       <c r="D105">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E105" t="str">
+        <f t="shared" si="5"/>
+        <v>G7</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>104</v>
       </c>
       <c r="B106" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3322.4375806395601</v>
       </c>
       <c r="C106" t="s">
         <v>12</v>
       </c>
       <c r="D106">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E106" t="str">
+        <f t="shared" si="5"/>
+        <v>G#7</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>105</v>
       </c>
       <c r="B107" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3520</v>
       </c>
       <c r="C107" t="s">
         <v>13</v>
       </c>
       <c r="D107">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E107" t="str">
+        <f t="shared" si="5"/>
+        <v>A7</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>106</v>
       </c>
       <c r="B108" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3729.3100921447194</v>
       </c>
       <c r="C108" t="s">
         <v>14</v>
       </c>
       <c r="D108">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E108" t="str">
+        <f t="shared" si="5"/>
+        <v>A#7</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>107</v>
       </c>
       <c r="B109" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3951.0664100489917</v>
       </c>
       <c r="C109" t="s">
         <v>15</v>
       </c>
       <c r="D109">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E109" t="str">
+        <f t="shared" si="5"/>
+        <v>B7</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>108</v>
       </c>
       <c r="B110" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4186.0090448095771</v>
       </c>
       <c r="C110" t="s">
         <v>4</v>
       </c>
       <c r="D110">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E110" t="str">
+        <f t="shared" si="5"/>
+        <v>C8</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>109</v>
       </c>
       <c r="B111" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4434.9220956299532</v>
       </c>
       <c r="C111" t="s">
@@ -2211,293 +2605,369 @@
         <f>D99+1</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E111" t="str">
+        <f t="shared" si="5"/>
+        <v>C#8</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>110</v>
       </c>
       <c r="B112" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4698.6362866785194</v>
       </c>
       <c r="C112" t="s">
         <v>6</v>
       </c>
       <c r="D112">
-        <f t="shared" ref="D112:D129" si="5">D100+1</f>
+        <f t="shared" ref="D112:D129" si="7">D100+1</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E112" t="str">
+        <f t="shared" si="5"/>
+        <v>D8</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>111</v>
       </c>
       <c r="B113" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4978.0317395532938</v>
       </c>
       <c r="C113" t="s">
         <v>7</v>
       </c>
       <c r="D113">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E113" t="str">
+        <f t="shared" si="5"/>
+        <v>D#8</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>112</v>
       </c>
       <c r="B114" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5274.0409106059187</v>
       </c>
       <c r="C114" t="s">
         <v>8</v>
       </c>
       <c r="D114">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E114" t="str">
+        <f t="shared" si="5"/>
+        <v>E8</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>113</v>
       </c>
       <c r="B115" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5587.6517029280612</v>
       </c>
       <c r="C115" t="s">
         <v>9</v>
       </c>
       <c r="D115">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E115" t="str">
+        <f t="shared" si="5"/>
+        <v>F8</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>114</v>
       </c>
       <c r="B116" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5919.9107633861504</v>
       </c>
       <c r="C116" t="s">
         <v>10</v>
       </c>
       <c r="D116">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E116" t="str">
+        <f t="shared" si="5"/>
+        <v>F#8</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>115</v>
       </c>
       <c r="B117" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6271.9269757079892</v>
       </c>
       <c r="C117" t="s">
         <v>11</v>
       </c>
       <c r="D117">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E117" t="str">
+        <f t="shared" si="5"/>
+        <v>G8</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>116</v>
       </c>
       <c r="B118" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6644.8751612791211</v>
       </c>
       <c r="C118" t="s">
         <v>12</v>
       </c>
       <c r="D118">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E118" t="str">
+        <f t="shared" si="5"/>
+        <v>G#8</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>117</v>
       </c>
       <c r="B119" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7040</v>
       </c>
       <c r="C119" t="s">
         <v>13</v>
       </c>
       <c r="D119">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E119" t="str">
+        <f t="shared" si="5"/>
+        <v>A8</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>118</v>
       </c>
       <c r="B120" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7458.6201842894361</v>
       </c>
       <c r="C120" t="s">
         <v>14</v>
       </c>
       <c r="D120">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E120" t="str">
+        <f t="shared" si="5"/>
+        <v>A#8</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>119</v>
       </c>
       <c r="B121" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7902.1328200979879</v>
       </c>
       <c r="C121" t="s">
         <v>15</v>
       </c>
       <c r="D121">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E121" t="str">
+        <f t="shared" si="5"/>
+        <v>B8</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>120</v>
       </c>
       <c r="B122" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8372.0180896191559</v>
       </c>
       <c r="C122" t="s">
         <v>4</v>
       </c>
       <c r="D122">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E122" t="str">
+        <f t="shared" si="5"/>
+        <v>C9</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>121</v>
       </c>
       <c r="B123" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8869.8441912599046</v>
       </c>
       <c r="C123" t="s">
         <v>5</v>
       </c>
       <c r="D123">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E123" t="str">
+        <f t="shared" si="5"/>
+        <v>C#9</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>122</v>
       </c>
       <c r="B124" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9397.2725733570442</v>
       </c>
       <c r="C124" t="s">
         <v>6</v>
       </c>
       <c r="D124">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E124" t="str">
+        <f t="shared" si="5"/>
+        <v>D9</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>123</v>
       </c>
       <c r="B125" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9956.0634791065877</v>
       </c>
       <c r="C125" t="s">
         <v>7</v>
       </c>
       <c r="D125">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E125" t="str">
+        <f t="shared" si="5"/>
+        <v>D#9</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>124</v>
       </c>
       <c r="B126" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10548.081821211836</v>
       </c>
       <c r="C126" t="s">
         <v>8</v>
       </c>
       <c r="D126">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E126" t="str">
+        <f t="shared" si="5"/>
+        <v>E9</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>125</v>
       </c>
       <c r="B127" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>11175.303405856126</v>
       </c>
       <c r="C127" t="s">
         <v>9</v>
       </c>
       <c r="D127">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E127" t="str">
+        <f t="shared" si="5"/>
+        <v>F9</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>126</v>
       </c>
       <c r="B128" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>11839.821526772301</v>
       </c>
       <c r="C128" t="s">
         <v>10</v>
       </c>
       <c r="D128">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E128" t="str">
+        <f t="shared" si="5"/>
+        <v>F#9</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>127</v>
       </c>
       <c r="B129" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12543.853951415975</v>
       </c>
       <c r="C129" t="s">
         <v>11</v>
       </c>
       <c r="D129">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>9</v>
+      </c>
+      <c r="E129" t="str">
+        <f t="shared" si="5"/>
+        <v>G9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>